<commit_message>
New design + add link + add description
</commit_message>
<xml_diff>
--- a/Organizations_V3.xlsx
+++ b/Organizations_V3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paren\Documents\RA\placedumarche_recengine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9322DE8F-ADA1-4EEA-AE77-C3E52FD7193D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A20D22-D0AC-4D4C-92C1-E2016B5BE3A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="14586" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="151">
   <si>
     <t>OrgID</t>
   </si>
@@ -80,9 +80,6 @@
     <t>garden, prep, cook, grocery store</t>
   </si>
   <si>
-    <t>La Maison de Quartier Villeray is a registered charity that has been established since 1989. It offers activities promoting the creation of bonds of mutual aid and solidarity between participants, with the aim of individual and collective empowerment. , which contributes to improving the living conditions of citizens.</t>
-  </si>
-  <si>
     <t>Resto Plateau</t>
   </si>
   <si>
@@ -98,9 +95,6 @@
     <t>prep, cook</t>
   </si>
   <si>
-    <t>A player in the social economy, Resto Plateau is a non-profit organization whose mission is to promote autonomy, inclusion and access to resources to meet essential needs such as food security, of the Montreal community and the surrounding area.</t>
-  </si>
-  <si>
     <t>MADA Community Center</t>
   </si>
   <si>
@@ -116,9 +110,6 @@
     <t>delivery, serve, warehouse</t>
   </si>
   <si>
-    <t>volunteer-based organization that evolved from a small neighbourhood centre to Montreal’s central address for fighting poverty in our community</t>
-  </si>
-  <si>
     <t>Mile End Mission</t>
   </si>
   <si>
@@ -131,9 +122,6 @@
     <t>prep, cook, sort, warehouse</t>
   </si>
   <si>
-    <t xml:space="preserve">Mile End Community Mission is a volunteer-run, not-for-profit organization and community centre working with members of the community who have been marginalized by society for a variety of reasons.  Our services are used by people of all ages, many of whom struggle with addiction, are in poverty and/or are homeless. </t>
-  </si>
-  <si>
     <t>Sun Youth Organization</t>
   </si>
   <si>
@@ -152,9 +140,6 @@
     <t>prep, cook, serve</t>
   </si>
   <si>
-    <t>We are a non-profit organization whose objective is to enable a better quality of life and support for individuals and families in the Parc-Extension district by developing a strong support network around various initiatives. aimed at food security and autonomy: collective kitchens, workshops, courses, distribution of food, training and social activities </t>
-  </si>
-  <si>
     <t>Partageons L'espoir</t>
   </si>
   <si>
@@ -167,9 +152,6 @@
     <t>prep, delivery, sort, grocery store, thrift store</t>
   </si>
   <si>
-    <t>Inspired by the vision of a vibrant community where everyone has the opportunity and the means to achieve their dreams, Share the Warmth's mission is to sow hope and dream in the community through quality programs aimed at the development and success of young people, access to healthy food and health for all and training and preparation for employment.</t>
-  </si>
-  <si>
     <t>West Island Mission</t>
   </si>
   <si>
@@ -191,9 +173,6 @@
     <t>grocery store, professional skills</t>
   </si>
   <si>
-    <t>The La Petite-Patrie Community Resource and Action Center (CRACPP) is an organization that fights against poverty. Through its food security activities and its fight against waste, it contributes to improving the living conditions of members of its community and to the defense of fundamental human rights.</t>
-  </si>
-  <si>
     <t>Le PAS de la Rue</t>
   </si>
   <si>
@@ -245,9 +224,6 @@
     <t>clean, cook, prep, serve</t>
   </si>
   <si>
-    <t>Robin des Bois is a non-profit restaurant. Our mission is to overcome loneliness, social isolation and poverty</t>
-  </si>
-  <si>
     <t>Moisson Rive Sud</t>
   </si>
   <si>
@@ -341,9 +317,6 @@
     <t>Organization Location</t>
   </si>
   <si>
-    <t>Moisson Rive-Sud is the main food bank of the south shore of Montreal. Covering more than 70% of the territory, it collects nearly 3.3 million Kg of food from companies and redistributes it free of charge to more than 100 organizations working with the vulnerable population.</t>
-  </si>
-  <si>
     <t>thrift store</t>
   </si>
   <si>
@@ -371,9 +344,6 @@
     <t>clean, cook, prep, delivery, sort</t>
   </si>
   <si>
-    <t>Since 1986, the Association des popotes roulantes du Montréal Métropolitain has been coordinating a network entirely volunteer run popotes. The Association promote the development of complementary services through strategic partnerships and collaborations.</t>
-  </si>
-  <si>
     <t>food security - women</t>
   </si>
   <si>
@@ -383,24 +353,9 @@
     <t>clean, cook, prep, delivery, sort, social assistance</t>
   </si>
   <si>
-    <t>Santropol Roulant is an intergenerational community food hub where we grow, prepare and deliver food. In doing so, we create a continuum of engaging services that help build a stronger social fabric, and increase food security and social inclusion for Montrealers.</t>
-  </si>
-  <si>
-    <t>The original purpose of The Yellow Door (at the time, YMCA of McGill), incorporated by a motion of Parliament in 1904, was to promote morality, religion, and social intercourse at the university. Later on, as the organization became more independent and the focus strayed from Christian values, our name was changed to The Yellow Door and the whole of the downtown core became our workplace. </t>
-  </si>
-  <si>
-    <t>Meals For Milton-Parc (M4MP) is a community-based project supporting the individuals without houses in the Milton-Parc neighborhood.</t>
-  </si>
-  <si>
-    <t>Chez Doris is a women’s shelter with the mandate to help any women in a position of difficulty.</t>
-  </si>
-  <si>
     <t>social assistance, education, daycare, sort, clean, cook, prep</t>
   </si>
   <si>
-    <t>Founded by Father Emmett Johns “Pops” in 1988, Dans la rue helps homeless and at-risk youth. With dedication, empathy and respect, and with the support of the community, Dans la rue cares for their immediate needs and helps them acquire the skills and ressources needed to lead more autonomous and rewarding lives.</t>
-  </si>
-  <si>
     <t>Midnight Kitchen is a non-profit, worker and volunteer-run collective that operates out of tio’tia:ke (unceded kanien’kehá:ka territory) dedicated to providing accessible food to as many people as possible.</t>
   </si>
   <si>
@@ -411,6 +366,117 @@
   </si>
   <si>
     <t>Saint Columba is engaged in seeking justice through empowerment, education and social action, as a community ministry of the United Church of Canada in partnership with the Point Saint Charles Community.</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>https://www.myplacedumarche.com/le-chic-resto-pop/</t>
+  </si>
+  <si>
+    <t>https://www.myplacedumarche.com/la-maison-de-quartier-villeray/</t>
+  </si>
+  <si>
+    <t>https://www.myplacedumarche.com/resto-plateau/</t>
+  </si>
+  <si>
+    <t>https://www.myplacedumarche.com/mada-community-center/</t>
+  </si>
+  <si>
+    <t>https://www.myplacedumarche.com/mile-end-community-mission/</t>
+  </si>
+  <si>
+    <t>https://www.myplacedumarche.com/sun-youth-organization/</t>
+  </si>
+  <si>
+    <t>https://www.myplacedumarche.com/cuisine-et-vie-collective-saint-roch/</t>
+  </si>
+  <si>
+    <t>https://www.myplacedumarche.com/partageons-lespoir/</t>
+  </si>
+  <si>
+    <t>https://www.myplacedumarche.com/west-island-mission/</t>
+  </si>
+  <si>
+    <t>https://www.myplacedumarche.com/centre-de-ressources-et-daction-communautaire-de-la-petite-patrie/</t>
+  </si>
+  <si>
+    <t>https://www.myplacedumarche.com/le-pas-de-la-rue/</t>
+  </si>
+  <si>
+    <t>https://www.myplacedumarche.com/robins-des-bois/</t>
+  </si>
+  <si>
+    <t>https://www.myplacedumarche.com/moisson-rive-sud/</t>
+  </si>
+  <si>
+    <t>https://www.myplacedumarche.com/chez-doris/</t>
+  </si>
+  <si>
+    <t>https://www.myplacedumarche.com/meals-for-milton-parc/</t>
+  </si>
+  <si>
+    <t>https://www.myplacedumarche.com/the-yellow-door/</t>
+  </si>
+  <si>
+    <t>https://www.myplacedumarche.com/santropol-roulant/</t>
+  </si>
+  <si>
+    <t>https://www.myplacedumarche.com/aprmm/</t>
+  </si>
+  <si>
+    <t>https://www.myplacedumarche.com/dans-la-rue/</t>
+  </si>
+  <si>
+    <t>https://www.myplacedumarche.com/midnight-kitchen/</t>
+  </si>
+  <si>
+    <t>https://www.myplacedumarche.com/saint-columba-house/</t>
+  </si>
+  <si>
+    <t>Robin des Bois is a non-profit restaurant. Our mission is to overcome loneliness, social isolation and poverty.</t>
+  </si>
+  <si>
+    <t>Chez Doris is a women’s shelter with the mandate to help any women in a position of difficulty.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meals For Milton-Parc (M4MP) is a community-based project supporting the individuals without houses in the Milton-Parc neighborhood. </t>
+  </si>
+  <si>
+    <t>Empower older adults and young people to initiate and engage in community and creative projects that promote social inclusion, combat urban isolation across all generations, and spark positive societal change.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Since 1986, the Association des popotes roulantes du Montréal Métropolitain (APRMM) has been coordinating a network of entirely volunteer run popotes. </t>
+  </si>
+  <si>
+    <t>Volunteer-based organization that evolved from a small neighbourhood centre to Montreal’s central address for fighting poverty in our community</t>
+  </si>
+  <si>
+    <t>Non-profit organization that aims to give a better life quality and support for people and families of the Parc-Extension neighbourhood.</t>
+  </si>
+  <si>
+    <t>Non-profit organization with the goal of increasing autonomy, inclusion, and access to resources by providing essential needs such as food security for Montréal community and its surrounding.</t>
+  </si>
+  <si>
+    <t>Our mission is to awaken hopes and dreams in the community through programs that fosters the overall development and success of youth, increases access to food security and health for all and offers work training programs.</t>
+  </si>
+  <si>
+    <t>Since 1989, It offers activities stimulating mutual aid and solidarity between its participants. Its goal is to support individuals while offering a collective environment that contributes to improving life conditions of citizens.</t>
+  </si>
+  <si>
+    <t>Non-profit organization that fight against poverty. Through activities in food security and and against waste, it improves life conditions of its members and defend their fundamental rights.</t>
+  </si>
+  <si>
+    <t>Focused on helping homeless and at-risk youth.  Dans la rue cares for their immediate needs and helps them acquire the skills and ressources needed to lead more autonomous and rewarding lives.</t>
+  </si>
+  <si>
+    <t>Volunteer-run, not-for-profit organization and community centre working with members of the community who have been marginalized by society for a variety of reasons. </t>
+  </si>
+  <si>
+    <t>Main food bank of the south shore of Montreal. Covering more than 70% of the territory, it collects nearly 3.3 million Kg of food from companies and redistributes it free of charge to more than 100 organizations working with the vulnerable population.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intergenerational community food hub where we grow, prepare and deliver food. We create a continuum of engaging services that help build a stronger social fabric, and increase food security and social inclusion for Montrealers. </t>
   </si>
 </sst>
 </file>
@@ -899,10 +965,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1258,10 +1329,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1271,10 +1342,10 @@
     <col min="5" max="5" width="14.05859375" customWidth="1"/>
     <col min="6" max="6" width="24.41015625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="40.703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.9375" customWidth="1"/>
+    <col min="8" max="8" width="15.9375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1299,8 +1370,11 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="I1" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1322,11 +1396,14 @@
       <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="I2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1348,120 +1425,135 @@
       <c r="G3" t="s">
         <v>17</v>
       </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="H3" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="I3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>22</v>
       </c>
-      <c r="G4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="H4" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="I4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
         <v>25</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
         <v>26</v>
       </c>
-      <c r="D5" t="s">
+      <c r="G5" t="s">
         <v>27</v>
       </c>
-      <c r="E5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="H5" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="I5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s">
         <v>31</v>
       </c>
-      <c r="C6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="H6" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="I6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F7" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="G7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.5">
+        <v>33</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
@@ -1473,206 +1565,230 @@
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G8" t="s">
-        <v>41</v>
-      </c>
-      <c r="H8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.5">
+        <v>37</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="I8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G9" t="s">
-        <v>46</v>
-      </c>
-      <c r="H9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.5">
+        <v>41</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F10" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G10" t="s">
-        <v>51</v>
-      </c>
-      <c r="H10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.5">
+        <v>45</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F11" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G11" t="s">
-        <v>54</v>
-      </c>
-      <c r="H11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.5">
+        <v>48</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F12" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G12" t="s">
-        <v>58</v>
-      </c>
-      <c r="H12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.5">
+        <v>51</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
         <v>20</v>
       </c>
-      <c r="D13" t="s">
-        <v>21</v>
-      </c>
       <c r="E13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G13" t="s">
-        <v>72</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.5">
+        <v>65</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="I13" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C14" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F14" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="G14" t="s">
         <v>12</v>
       </c>
-      <c r="H14" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="H14" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="I14" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F15" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G15" t="s">
-        <v>107</v>
-      </c>
-      <c r="H15" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.5">
+        <v>98</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="I15" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D16" t="s">
         <v>10</v>
@@ -1681,128 +1797,143 @@
         <v>10</v>
       </c>
       <c r="F16" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="G16" t="s">
-        <v>108</v>
-      </c>
-      <c r="H16" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.5">
+        <v>99</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="I16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F17" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G17" t="s">
-        <v>113</v>
-      </c>
-      <c r="H17" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.5">
+        <v>104</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="I17" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" t="s">
         <v>20</v>
       </c>
-      <c r="D18" t="s">
-        <v>21</v>
-      </c>
       <c r="E18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F18" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G18" t="s">
-        <v>118</v>
-      </c>
-      <c r="H18" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.5">
+        <v>108</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="I18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C19" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D19" t="s">
         <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F19" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G19" t="s">
-        <v>114</v>
-      </c>
-      <c r="H19" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.5">
+        <v>105</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="I19" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F20" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G20" t="s">
-        <v>123</v>
-      </c>
-      <c r="H20" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.5">
+        <v>109</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="I20" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D21" t="s">
         <v>10</v>
@@ -1811,40 +1942,49 @@
         <v>10</v>
       </c>
       <c r="F21" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G21" t="s">
-        <v>126</v>
-      </c>
-      <c r="H21" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.5">
+        <v>111</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="I21" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C22" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F22" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G22" t="s">
-        <v>127</v>
-      </c>
-      <c r="H22" t="s">
-        <v>128</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I22" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="H27" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1867,87 +2007,87 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1971,32 +2111,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2019,47 +2159,47 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.5">
@@ -2069,7 +2209,7 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.5">
@@ -2079,37 +2219,37 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix recommendation bug with localisation
</commit_message>
<xml_diff>
--- a/Organizations_V3.xlsx
+++ b/Organizations_V3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paren\Documents\RA\placedumarche_recengine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A20D22-D0AC-4D4C-92C1-E2016B5BE3A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03610B39-2A01-4A37-BAB3-5B1E8B0E8519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="14586" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="152">
   <si>
     <t>OrgID</t>
   </si>
@@ -477,6 +477,9 @@
   </si>
   <si>
     <t xml:space="preserve">Intergenerational community food hub where we grow, prepare and deliver food. We create a continuum of engaging services that help build a stronger social fabric, and increase food security and social inclusion for Montrealers. </t>
+  </si>
+  <si>
+    <t>Le Sud-Ouest</t>
   </si>
 </sst>
 </file>
@@ -1332,7 +1335,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1585,7 +1588,7 @@
         <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>86</v>
+        <v>151</v>
       </c>
       <c r="D9" t="s">
         <v>25</v>
@@ -1875,7 +1878,7 @@
         <v>71</v>
       </c>
       <c r="C19" t="s">
-        <v>86</v>
+        <v>151</v>
       </c>
       <c r="D19" t="s">
         <v>10</v>
@@ -1962,7 +1965,7 @@
         <v>74</v>
       </c>
       <c r="C22" t="s">
-        <v>86</v>
+        <v>151</v>
       </c>
       <c r="D22" t="s">
         <v>25</v>

</xml_diff>